<commit_message>
Connect data throughout classes
</commit_message>
<xml_diff>
--- a/writtenExcelFile.xlsx
+++ b/writtenExcelFile.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Student Name</t>
   </si>
@@ -32,7 +32,7 @@
     <t>End Date</t>
   </si>
   <si>
-    <t>Tom Jones</t>
+    <t>Kenny Imarah</t>
   </si>
   <si>
     <t>tom@willis.com</t>
@@ -48,30 +48,6 @@
   </si>
   <si>
     <t>18-01-2020</t>
-  </si>
-  <si>
-    <t>Jane Keene</t>
-  </si>
-  <si>
-    <t>jane@willis.com</t>
-  </si>
-  <si>
-    <t>Trip Advisor</t>
-  </si>
-  <si>
-    <t>David Andrews</t>
-  </si>
-  <si>
-    <t>david@willis.com</t>
-  </si>
-  <si>
-    <t>Sandra Li</t>
-  </si>
-  <si>
-    <t>sandra@willis.com</t>
-  </si>
-  <si>
-    <t>Government of Canada</t>
   </si>
 </sst>
 </file>
@@ -123,7 +99,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -169,66 +145,6 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>